<commit_message>
ArrayFeature done except practice questions
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/PythonData.xlsx
+++ b/src/test/resources/exceldata/PythonData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C060D3B6-1229-4C1E-AE4E-2756DA66F759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FF83D044-B072-4423-8614-846FA5C5D365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19400" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>pythonCode</t>
   </si>
@@ -34,6 +34,28 @@
 print ("Index of Ford is" ,IndexOfFord)
 for x in cars:
   print(x)</t>
+  </si>
+  <si>
+    <t>grocery = ["apples", "bananas", "cucumbers", "dates", "strawberries"]
+grocery.append("oranges")
+for fruits in grocery:
+  print(fruits)</t>
+  </si>
+  <si>
+    <t>grocery_list = ["apples", "bananas", "cucumbers", "dates", "strawberries"]
+grocery_list.insert(2,"cashews")
+grocery_list.pop()
+for list in grocery_list:
+  print(list)</t>
+  </si>
+  <si>
+    <t>marks = [3, 5, 4, 2, 5, 5, 3, 5, 4, 4, 4]
+sum_of_marks=sum(marks)
+len_of_marks=len(marks)
+print(sum_of_marks)
+print(len_of_marks)
+result = sum(marks) / len(marks)
+print("The final grade:" + str(result))</t>
   </si>
 </sst>
 </file>
@@ -354,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A8:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,7 +399,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>